<commit_message>
change the registration page
</commit_message>
<xml_diff>
--- a/JTSMS.xlsx
+++ b/JTSMS.xlsx
@@ -5,20 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1099969\Desktop\Development\GitHub\JTSMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1099969\Desktop\Development\GitHub\JTSMS_v2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0362BBE0-CA54-48C9-9297-797366E34C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF9E52E-096D-40B7-94D3-2440F6D86C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="806" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="806" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DatabaseTable Old Version" sheetId="1" r:id="rId1"/>
-    <sheet name="DatabaseTable" sheetId="6" r:id="rId2"/>
-    <sheet name="Pages" sheetId="3" r:id="rId3"/>
-    <sheet name="WatchdogConfig Page" sheetId="4" r:id="rId4"/>
-    <sheet name="Function" sheetId="2" r:id="rId5"/>
-    <sheet name="Registration Page" sheetId="5" r:id="rId6"/>
+    <sheet name="Enhancement" sheetId="7" r:id="rId1"/>
+    <sheet name="Registration Page" sheetId="5" r:id="rId2"/>
+    <sheet name="TC" sheetId="8" r:id="rId3"/>
+    <sheet name="DatabaseTable" sheetId="6" r:id="rId4"/>
+    <sheet name="DatabaseTable Old Version" sheetId="1" r:id="rId5"/>
+    <sheet name="Pages" sheetId="3" r:id="rId6"/>
+    <sheet name="WatchdogConfig Page" sheetId="4" r:id="rId7"/>
+    <sheet name="Function" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="250">
   <si>
     <t>ticketId</t>
   </si>
@@ -537,12 +539,6 @@
     <t>Family</t>
   </si>
   <si>
-    <t>is used for Multiple Assy#</t>
-  </si>
-  <si>
-    <t>isCommon?</t>
-  </si>
-  <si>
     <t>Created By</t>
   </si>
   <si>
@@ -606,14 +602,267 @@
     <t>isReady</t>
   </si>
   <si>
-    <t>number</t>
+    <t>Button Copy test script ID to clipboard</t>
+  </si>
+  <si>
+    <t>Image attachment for evidence</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>Scrip Id</t>
+  </si>
+  <si>
+    <t>Assy1</t>
+  </si>
+  <si>
+    <t>Assy2</t>
+  </si>
+  <si>
+    <t>Assy3</t>
+  </si>
+  <si>
+    <t>Assy4</t>
+  </si>
+  <si>
+    <t>Assy5</t>
+  </si>
+  <si>
+    <t>script id1</t>
+  </si>
+  <si>
+    <t>script id2</t>
+  </si>
+  <si>
+    <t>reqId1</t>
+  </si>
+  <si>
+    <t>reqId2</t>
+  </si>
+  <si>
+    <t>reqId3</t>
+  </si>
+  <si>
+    <t>Assy6</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>testscript</t>
+  </si>
+  <si>
+    <t>testscript'</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>PCN</t>
+  </si>
+  <si>
+    <t>script id3</t>
+  </si>
+  <si>
+    <t>Request Number</t>
+  </si>
+  <si>
+    <t>A button next to the script ID for user to copy the script ID to the clipboard</t>
+  </si>
+  <si>
+    <t>Allow user to attached images as their change detail evidences and approvers are able to download and view the attachment
+- Save image in path: VNHCMM0TEAPP05/JTSMS/Attachment/Evidence/customer/process/assembly
+- Can add multiple images
+- user can download and view images</t>
+  </si>
+  <si>
+    <t>Store the test scipts base on customer/process/family/assembly. Allow user to run the test script to be called by the test station</t>
+  </si>
+  <si>
+    <t>if the test script is for multiple assy#, store it for each assembly number folder in the server
+Path: 
+- VNHCMM0TEAPP05/JTSMS/Attachment/Encrypted/customer/process/assembly
+- VNHCMM0TEAPP05/JTSMS/Attachment/Origin/customer/process/assembly
+- vnhcmm0src03/JTSMS/Attachment/Encrypted/customer/process/assembly</t>
+  </si>
+  <si>
+    <t>Add Assembly Test Properties Page</t>
+  </si>
+  <si>
+    <t>Allow user to add Assembly Test Properties and store the JTSMS DB:
+- Type 1: Measurement Properties - KeyName, Lower Limit, Upper Limit, Measurement Unit.
+- Type 2: Information Properties - KeyName, Value.
+	Allow user to add/change mutiple configuration files and generate the configuration file HASH string same as test script file hash string.
+	VNHCMM0TEAPP05/JTSMS/Attachment/Configuration/customer/process/assembly
+	Create an approval loop same as test script change approval loop after clicking on submit button</t>
+  </si>
+  <si>
+    <t>Add Report Pages</t>
+  </si>
+  <si>
+    <t>Assembly Number activity log (list of request of particular Assy#)
+	Report SN using system with Customer filter, process filter, time frame filter - (Customer, Process, Assembly Number, Serial Number, Equipment, Script File Name, Validation result, User, Record date).
+	report SN using un-verified test script with Customer filter, process filter, time frame filter - (Customer, Process, Assembly Number, Serial Number, Equipment, MES Start Test Date, Record date).
+	report testers using watchdog with Customer filter, process filter - (Customer, Process, EquipmetName, User added, Record Date).
+	report testers which are not using watch dog with Customer filter, process filter - (Customer, Process, EquipmetName)</t>
+  </si>
+  <si>
+    <t>Multiple Assy# using same script ID</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>script id4</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ECN</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Number of Assy#</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>TC Number</t>
+  </si>
+  <si>
+    <t>There should be a link to the new section that allows users to add computers to the database</t>
+  </si>
+  <si>
+    <t>Actual Results / Comments:</t>
+  </si>
+  <si>
+    <t>- Open the web browser
+- Navigate to the computer database app
+- should see a new button called "Add a New Computer"</t>
+  </si>
+  <si>
+    <t>1. Access the computer database app
+2. the list of the item is showing in the table and there is a column called "Computer Name"
+3. click on the link in "Computer Name" column, a new section will be show to update the database
+4. The new section should have a heading of "Add a New Computer"</t>
+  </si>
+  <si>
+    <t>1. Access the computer database app
+2. navigate to the new section using the button link
+3. four fields labelled"&lt;fields&gt;" with a type of "&lt;type&gt;" will be shown
+      |    type    |      fields       |
+      | Free input |   Computer Name   |
+      | Free input |  Introduced Date  |
+      | Free input | Discontinued Date |
+      | Free Input |   Manufacturer    |
+4. two buttons named "&lt;buttons&gt;" will be shown:
+      | Add Computer |
+      |    Cancel    |</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>It Should allow me to cancel the operation
+1. It should take me back to the main computer database view</t>
+  </si>
+  <si>
+    <t>1. entering a new computer into the system
+2. click "Cancel" button</t>
+  </si>
+  <si>
+    <t>The app is shown
+There is a button "Add a New Computer" near the top-right corner</t>
+  </si>
+  <si>
+    <t>It should be possible to open the new section
+1. list of item is showing
+2. new section will show once click on single item</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. the app is accessible
+2. list item show
+3. section is show after clicking item 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4. there is no heading called "Add a New Computer", but "Edit computer" is showing</t>
+    </r>
+  </si>
+  <si>
+    <t>It should have four new fields and two buttons in the new section
+1. the app is accessible
+2. new section will be shown after clicking in the link
+3. Computer Name, Introduced Date, Discontinued Date and Manufacturer field will be shown
+4. 2 buttons are showing (Add Computer and Cancel)</t>
+  </si>
+  <si>
+    <t>1. the app is accessible
+2. new section will be shown after clicking in the link
+3. Computer Name, Introduced Date, Discontinued Date and Manufacturer field is shown
+4. Cancel button is shown, but Add Computer is not shown</t>
+  </si>
+  <si>
+    <t>1. back to the main app database after clicking Cancel</t>
+  </si>
+  <si>
+    <t>1. Click on "Add a New Computer", it will navigate to new section
+2. only entered a name for a computer
+3. click "Add This Computer" 
+4. It indicate which fields are mandatory</t>
+  </si>
+  <si>
+    <t>It should not allow new computers to be added unless all fields are populated
+1. data is not saved and It should indicate which fields are mandatory</t>
+  </si>
+  <si>
+    <t>1. data is saved and It back to main app</t>
+  </si>
+  <si>
+    <t>Pending submission</t>
+  </si>
+  <si>
+    <t>approved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,6 +890,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -794,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -856,11 +1117,49 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1156,846 +1455,605 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:T59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BF485C-D1E7-4862-9488-3EEA72BE3375}">
+  <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="1" t="s">
+    <row r="2" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="37">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40">
+        <v>44727</v>
+      </c>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="37">
+        <v>2</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="2:8" s="17" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="B5" s="37">
         <v>3</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="C5" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="2:8" s="17" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="B6" s="37">
+        <v>4</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="2:8" s="17" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="B7" s="37"/>
+      <c r="C7" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="2:8" s="17" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="B8" s="37"/>
+      <c r="C8" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="4"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD64A3-63F1-40B3-90EB-5A42BF3D1EC5}">
+  <dimension ref="A2:X34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.26953125" style="30" customWidth="1"/>
+    <col min="9" max="10" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.6328125" style="31" customWidth="1"/>
+    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6328125" customWidth="1"/>
+    <col min="21" max="21" width="8.54296875" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="E2" s="43"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" s="32"/>
+      <c r="I6" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="U6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="W6" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="X6" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="M7" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O7" t="s">
+        <v>188</v>
+      </c>
+      <c r="P7" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>189</v>
+      </c>
+      <c r="R7" t="s">
+        <v>189</v>
+      </c>
+      <c r="S7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="W7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="X7" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B8" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B10" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="17">
+        <v>1</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
-        <v>2</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="17">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="I11" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B12" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="P16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="30"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1099969</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1099969</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
+      <c r="F21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J21" s="30"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="30"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="30"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>1</v>
-      </c>
-      <c r="M24" t="s">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>21</v>
-      </c>
-      <c r="R24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>2</v>
+        <v>206</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="30"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25" t="str">
-        <f>VLOOKUP(O25,A23:B26,2,0)</f>
-        <v>Superior</v>
-      </c>
-      <c r="S25">
-        <f>VLOOKUP(P25,A30:C34,3,0)</f>
-        <v>1099969</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>14</v>
-      </c>
-      <c r="M26" t="s">
-        <v>15</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>2</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26" t="str">
-        <f>VLOOKUP(O26,A24:B26,2,0)</f>
-        <v>Superior</v>
-      </c>
-      <c r="S26" t="str">
-        <f>VLOOKUP(P26,A31:C35,3,0)</f>
-        <v>quochuyn</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" t="s">
-        <v>15</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>2</v>
-      </c>
-      <c r="P27">
-        <v>3</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27" t="str">
-        <f>VLOOKUP(O27,A25:B26,2,0)</f>
-        <v>Lead Approval</v>
-      </c>
-      <c r="S27" t="str">
-        <f>VLOOKUP(P27,A32:C35,3,0)</f>
-        <v>edwinA</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M28" t="s">
-        <v>15</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28">
-        <v>3</v>
-      </c>
-      <c r="P28">
-        <v>4</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28" t="str">
-        <f>VLOOKUP(O28,A26:B29,2,0)</f>
-        <v>SME Lead Approval</v>
-      </c>
-      <c r="S28" t="str">
-        <f>VLOOKUP(P28,A33:C35,3,0)</f>
-        <v>edwinM</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1099969</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N53" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
+        <v>197</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" t="s">
+        <v>249</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="30"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="30"/>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J27" s="30"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="30"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" t="s">
+        <v>221</v>
+      </c>
+      <c r="I31"/>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B33" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" s="30"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B34" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="F34" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H34" t="s">
+        <v>222</v>
+      </c>
+      <c r="I34"/>
+      <c r="J34" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2004,18 +2062,143 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70849DB-53E8-4BB5-BAFF-2B98EB4C492D}">
+  <dimension ref="A6:E11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" style="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18">
+        <v>1</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18">
+        <v>3</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="35">
+        <v>4</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="17" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18">
+        <v>5</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77C8594-E0BC-438D-A1AA-2C377D953E6A}">
   <dimension ref="A3:AB17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.26953125" style="17" bestFit="1" customWidth="1"/>
@@ -2064,13 +2247,13 @@
         <v>92</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>182</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="H4" s="35" t="s">
         <v>73</v>
@@ -2088,7 +2271,7 @@
         <v>100</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N4" s="18" t="s">
         <v>33</v>
@@ -2097,10 +2280,10 @@
         <v>34</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="R4" s="18" t="s">
         <v>35</v>
@@ -2153,86 +2336,935 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K10" s="34"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="D17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="E17" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="F17" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="G17" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="H17" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="I17" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="I17" s="36" t="s">
+      <c r="J17" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="36" t="s">
+      <c r="L17" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="36" t="s">
+      <c r="M17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="M17" s="36" t="s">
+      <c r="N17" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="36" t="s">
+      <c r="O17" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="36" t="s">
-        <v>185</v>
-      </c>
       <c r="P17" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q17" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="Q17" s="36" t="s">
+      <c r="R17" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="R17" s="36" t="s">
+      <c r="S17" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="T17" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="V17" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="W17" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="S17" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="T17" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U17" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="V17" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="W17" s="36" t="s">
+      <c r="X17" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="X17"/>
-      <c r="Z17" s="17"/>
-      <c r="AB17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:T59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1099969</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1099969</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>3</v>
+      </c>
+      <c r="O24" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25" t="str">
+        <f>VLOOKUP(O25,A23:B26,2,0)</f>
+        <v>Superior</v>
+      </c>
+      <c r="S25">
+        <f>VLOOKUP(P25,A30:C34,3,0)</f>
+        <v>1099969</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26" t="str">
+        <f>VLOOKUP(O26,A24:B26,2,0)</f>
+        <v>Superior</v>
+      </c>
+      <c r="S26" t="str">
+        <f>VLOOKUP(P26,A31:C35,3,0)</f>
+        <v>quochuyn</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27" t="str">
+        <f>VLOOKUP(O27,A25:B26,2,0)</f>
+        <v>Lead Approval</v>
+      </c>
+      <c r="S27" t="str">
+        <f>VLOOKUP(P27,A32:C35,3,0)</f>
+        <v>edwinA</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>3</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28" t="str">
+        <f>VLOOKUP(O28,A26:B29,2,0)</f>
+        <v>SME Lead Approval</v>
+      </c>
+      <c r="S28" t="str">
+        <f>VLOOKUP(P28,A33:C35,3,0)</f>
+        <v>edwinM</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1099969</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B54D99C-AB77-48B1-90F1-F2D1AF4920E5}">
   <dimension ref="B3:Q21"/>
   <sheetViews>
@@ -2615,7 +3647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EF34FF-B833-4FF0-BF1F-F9DACB0F9D04}">
   <dimension ref="B3:K3"/>
   <sheetViews>
@@ -2675,12 +3707,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6091898B-187E-4EBA-A7A0-8892F3E0AD79}">
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3081,134 +4113,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD64A3-63F1-40B3-90EB-5A42BF3D1EC5}">
-  <dimension ref="B4:V17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.26953125" style="30" customWidth="1"/>
-    <col min="10" max="10" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6328125" style="31" customWidth="1"/>
-    <col min="14" max="14" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.6328125" customWidth="1"/>
-    <col min="20" max="20" width="8.54296875" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="P6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="H7" t="s">
-        <v>164</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>175</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="O16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
migrate to new database
</commit_message>
<xml_diff>
--- a/JTSMS.xlsx
+++ b/JTSMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1099969\Desktop\Development\GitHub\JTSMS_v2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF9E52E-096D-40B7-94D3-2440F6D86C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F87BCD9-F8C0-4B40-B1CA-FFC7934BEB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="806" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2580" yWindow="2630" windowWidth="14400" windowHeight="7460" tabRatio="806" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enhancement" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="258">
   <si>
     <t>ticketId</t>
   </si>
@@ -681,9 +681,6 @@
 - Save image in path: VNHCMM0TEAPP05/JTSMS/Attachment/Evidence/customer/process/assembly
 - Can add multiple images
 - user can download and view images</t>
-  </si>
-  <si>
-    <t>Store the test scipts base on customer/process/family/assembly. Allow user to run the test script to be called by the test station</t>
   </si>
   <si>
     <t>if the test script is for multiple assy#, store it for each assembly number folder in the server
@@ -856,6 +853,33 @@
   </si>
   <si>
     <t>approved</t>
+  </si>
+  <si>
+    <t>now in Test folder</t>
+  </si>
+  <si>
+    <t>Store the test scripts based on customer/process/family/assembly. Allow user to run the test script to be called by the test station</t>
+  </si>
+  <si>
+    <t>Worcell selection based on granted</t>
+  </si>
+  <si>
+    <t>- Still need to check the condition before adding the Assy# to the database</t>
+  </si>
+  <si>
+    <t>- Need to test the file storage in mapping disk</t>
+  </si>
+  <si>
+    <t>Approval Flow</t>
+  </si>
+  <si>
+    <t>Customer Dropdown list will be shown based on what has been granted to the user</t>
+  </si>
+  <si>
+    <t>Show approval history of the request with detail status</t>
+  </si>
+  <si>
+    <t>whatchdog history</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1120,15 +1144,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1147,6 +1162,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1456,16 +1501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BF485C-D1E7-4862-9488-3EEA72BE3375}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" style="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.08984375" customWidth="1"/>
     <col min="7" max="7" width="13.90625" customWidth="1"/>
     <col min="8" max="8" width="16.7265625" customWidth="1"/>
   </cols>
@@ -1497,92 +1544,146 @@
       <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40">
+      <c r="F3" s="46"/>
+      <c r="G3" s="47">
         <v>44727</v>
       </c>
-      <c r="H3" s="39"/>
-    </row>
-    <row r="4" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="46"/>
+    </row>
+    <row r="4" spans="2:8" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="37">
         <v>2</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="39"/>
+      <c r="C4" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="49" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="47"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="2:8" s="17" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="B5" s="37">
         <v>3</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" s="50">
+        <v>44760</v>
+      </c>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="2:8" s="17" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="B6" s="37">
         <v>4</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="50"/>
+      <c r="H6" s="48"/>
+    </row>
+    <row r="7" spans="2:8" s="17" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="B7" s="37">
+        <v>5</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="2:8" s="17" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="B7" s="37"/>
-      <c r="C7" s="41" t="s">
+      <c r="D7" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="E7" s="52"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="48"/>
+    </row>
+    <row r="8" spans="2:8" s="17" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="37">
+        <v>6</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="2:8" s="17" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="B8" s="37"/>
-      <c r="C8" s="41" t="s">
+      <c r="D8" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="4"/>
       <c r="G8" s="21"/>
       <c r="H8" s="4"/>
     </row>
+    <row r="9" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="37"/>
+      <c r="C9" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C13" s="54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C14" s="54" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E4">
+  <conditionalFormatting sqref="E2:E3">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -1595,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD64A3-63F1-40B3-90EB-5A42BF3D1EC5}">
   <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1726,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="E2" s="43"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -1665,7 +1766,7 @@
         <v>165</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M6" s="18" t="s">
         <v>127</v>
@@ -1742,7 +1843,7 @@
         <v>202</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1763,7 +1864,7 @@
         <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1783,7 +1884,7 @@
         <v>202</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
@@ -1803,7 +1904,7 @@
         <v>202</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D11" s="17">
         <v>1</v>
@@ -1823,7 +1924,7 @@
         <v>202</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="17">
         <v>1</v>
@@ -1876,7 +1977,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1940,7 +2041,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2004,7 +2105,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -2015,13 +2116,13 @@
         <v>200</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>191</v>
       </c>
       <c r="H31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I31"/>
       <c r="J31" s="30"/>
@@ -2043,14 +2144,14 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C34" s="17"/>
       <c r="F34" s="17" t="s">
         <v>191</v>
       </c>
       <c r="H34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I34"/>
       <c r="J34" s="30"/>
@@ -2081,104 +2182,104 @@
   <sheetData>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>1</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>239</v>
+      <c r="B7" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>2</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>240</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="46" t="s">
+      <c r="B9" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="D9" s="46" t="s">
-        <v>243</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>240</v>
+      <c r="E9" s="43" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="35">
         <v>4</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="D10" s="44" t="s">
         <v>246</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>240</v>
+      <c r="E10" s="43" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="17" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>5</v>
       </c>
-      <c r="B11" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" s="46" t="s">
+      <c r="B11" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>239</v>
+      <c r="C11" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2439,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17" s="36" t="s">
         <v>45</v>

</xml_diff>